<commit_message>
added saving of figure and removed print line #noob
</commit_message>
<xml_diff>
--- a/computational study/comp_study_summary.xlsx
+++ b/computational study/comp_study_summary.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Comp study" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,363 +474,18 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03149</v>
+        <v>0.00053</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00104</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.00311</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.00314</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.05238</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.00052</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>10</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.00165</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>15</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.00301</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.00047</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1e+100</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.00215</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.01762</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>15</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.01736</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>20</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.00168</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" t="n">
-        <v>5</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.00277</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="n">
-        <v>20</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.0297</v>
-      </c>
-      <c r="G17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>